<commit_message>
ci-build 0.2.1 (#286) 9484b688ee3b621c3960f09c029910ea90f65298
</commit_message>
<xml_diff>
--- a/ig/main/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/ig/main/CodeSystem-act-type-ror-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.2.0</t>
+    <t>0.2.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-12T09:07:50+00:00</t>
+    <t>2024-01-12T15:06:45+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>